<commit_message>
Module : pabi_procurement_report FI : ปรับแก้ไขรายงานเปรียบเทียบใบขอซื้อและใบสั่งซื้อ (PR and PO Comparison) Issues : https://mobileapp.nstda.or.th/redmine/issues/3668
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_comparison_pr_po.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_comparison_pr_po.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NSTDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="3420" windowWidth="22480" windowHeight="10000" tabRatio="500"/>
+    <workbookView xWindow="4425" yWindow="3420" windowWidth="22485" windowHeight="10005" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>NSTDA</t>
   </si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Total Amount</t>
+  </si>
+  <si>
+    <t>PR Date</t>
   </si>
 </sst>
 </file>
@@ -83,7 +83,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -156,6 +156,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -424,65 +427,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -490,33 +500,37 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>